<commit_message>
Werte in Excel korrigiert, Aufgabe 1 korrigiert
</commit_message>
<xml_diff>
--- a/Ex1_2.2&3_noDamping.xlsx
+++ b/Ex1_2.2&3_noDamping.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\B\OneDrive\ETH\Physically-based Simulations in CG\Exercises\Ex1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benja\OneDrive\ETH\Physically-based Simulations in CG\Exercises\Ex1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="16">
   <si>
     <t>step</t>
   </si>
@@ -538,27 +538,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G69" sqref="G69:M71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="6" width="15.625" customWidth="1"/>
-    <col min="7" max="7" width="3.625" customWidth="1"/>
-    <col min="8" max="12" width="15.625" customWidth="1"/>
-    <col min="13" max="13" width="3.625" customWidth="1"/>
-    <col min="14" max="20" width="15.625" customWidth="1"/>
+    <col min="1" max="6" width="15.59765625" customWidth="1"/>
+    <col min="7" max="7" width="3.59765625" customWidth="1"/>
+    <col min="8" max="12" width="15.59765625" customWidth="1"/>
+    <col min="13" max="13" width="3.59765625" customWidth="1"/>
+    <col min="14" max="20" width="15.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:17" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="1:17" s="15" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="14" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" s="13" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -581,7 +581,7 @@
       <c r="P4" s="5"/>
       <c r="Q4" s="5"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A5" s="4" t="s">
         <v>0</v>
       </c>
@@ -628,40 +628,40 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
-        <v>3.0000000000000001E-3</v>
+        <v>0.5</v>
       </c>
       <c r="B6" s="1">
-        <v>-1.5901100000000001E-2</v>
+        <v>-2.6501800000000002</v>
       </c>
       <c r="C6" s="1">
-        <v>-1.5901100000000001E-2</v>
+        <v>-2.6501800000000002</v>
       </c>
       <c r="D6" s="1">
-        <v>-1.5529599999999999E-2</v>
+        <v>7.6683500000000002</v>
       </c>
       <c r="E6" s="1">
-        <v>-1.51445E-2</v>
+        <v>0.69180399999999997</v>
       </c>
       <c r="F6" s="1">
-        <v>-1.5527300000000001E-2</v>
+        <v>1.0995900000000001</v>
       </c>
       <c r="H6" s="1">
         <f>ABS(B6-F6)</f>
-        <v>3.7380000000000052E-4</v>
+        <v>3.7497700000000003</v>
       </c>
       <c r="I6" s="1">
         <f>ABS(C6-F6)</f>
-        <v>3.7380000000000052E-4</v>
+        <v>3.7497700000000003</v>
       </c>
       <c r="J6" s="1">
         <f>ABS(D6-F6)</f>
-        <v>2.2999999999984838E-6</v>
+        <v>6.5687600000000002</v>
       </c>
       <c r="K6" s="1">
         <f>ABS(E6-F6)</f>
-        <v>3.8280000000000085E-4</v>
+        <v>0.40778600000000009</v>
       </c>
       <c r="L6" s="1">
         <f>ABS(F6-F6)</f>
@@ -669,55 +669,55 @@
       </c>
       <c r="N6">
         <f>IF(H7=0,"",H6/H7)</f>
-        <v>4.0124516960068703</v>
+        <v>1.5031005856439077</v>
       </c>
       <c r="O6">
         <f t="shared" ref="O6:Q14" si="0">IF(I7=0,"",I6/I7)</f>
-        <v>4.0124516960068703</v>
+        <v>1.5031005856439077</v>
       </c>
       <c r="P6">
         <f t="shared" si="0"/>
-        <v>7.9310344827530512</v>
+        <v>77.334118201083101</v>
       </c>
       <c r="Q6">
         <f t="shared" si="0"/>
-        <v>4.0585241730279913</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.63642180701305362</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
-        <v>1.5E-3</v>
+        <v>0.25</v>
       </c>
       <c r="B7" s="1">
-        <v>-7.9505500000000007E-3</v>
+        <v>-1.3250900000000001</v>
       </c>
       <c r="C7" s="1">
-        <v>-7.9505500000000007E-3</v>
+        <v>-1.3250900000000001</v>
       </c>
       <c r="D7" s="1">
-        <v>-7.8576800000000006E-3</v>
+        <v>1.25454</v>
       </c>
       <c r="E7" s="1">
-        <v>-7.7630700000000004E-3</v>
+        <v>0.52885199999999999</v>
       </c>
       <c r="F7" s="1">
-        <v>-7.8573900000000006E-3</v>
+        <v>1.1696</v>
       </c>
       <c r="H7" s="1">
         <f t="shared" ref="H7:H15" si="1">ABS(B7-F7)</f>
-        <v>9.3160000000000118E-5</v>
+        <v>2.4946900000000003</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" ref="I7:I15" si="2">ABS(C7-F7)</f>
-        <v>9.3160000000000118E-5</v>
+        <v>2.4946900000000003</v>
       </c>
       <c r="J7" s="1">
         <f t="shared" ref="J7:J15" si="3">ABS(D7-F7)</f>
-        <v>2.9000000000001247E-7</v>
+        <v>8.4940000000000015E-2</v>
       </c>
       <c r="K7" s="1">
         <f t="shared" ref="K7:K15" si="4">ABS(E7-F7)</f>
-        <v>9.4320000000000168E-5</v>
+        <v>0.64074799999999998</v>
       </c>
       <c r="L7" s="1">
         <f t="shared" ref="L7:L15" si="5">ABS(F7-F7)</f>
@@ -725,55 +725,55 @@
       </c>
       <c r="N7">
         <f t="shared" ref="N7:N14" si="6">IF(H8=0,"",H7/H8)</f>
-        <v>4.006881720429992</v>
+        <v>3.4421899629549508</v>
       </c>
       <c r="O7">
         <f t="shared" si="0"/>
-        <v>4.006881720429992</v>
+        <v>3.4421899629549508</v>
       </c>
       <c r="P7">
         <f t="shared" si="0"/>
-        <v>7.2499999998861586</v>
+        <v>1.0640070249015727</v>
       </c>
       <c r="Q7">
         <f t="shared" si="0"/>
-        <v>4.0307692307692706</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+        <v>3.5091059049550974</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
-        <v>7.5000000000000002E-4</v>
+        <v>0.125</v>
       </c>
       <c r="B8" s="1">
-        <v>-3.9752700000000004E-3</v>
+        <v>-0.66254599999999997</v>
       </c>
       <c r="C8" s="1">
-        <v>-3.9752700000000004E-3</v>
+        <v>-0.66254599999999997</v>
       </c>
       <c r="D8" s="1">
-        <v>-3.9520600000000003E-3</v>
+        <v>-1.7637099999999999E-2</v>
       </c>
       <c r="E8" s="1">
-        <v>-3.9286199999999999E-3</v>
+        <v>0.24478900000000001</v>
       </c>
       <c r="F8" s="1">
-        <v>-3.9520199999999997E-3</v>
+        <v>6.2193199999999997E-2</v>
       </c>
       <c r="H8" s="1">
         <f t="shared" si="1"/>
-        <v>2.3250000000000701E-5</v>
+        <v>0.72473919999999992</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="2"/>
-        <v>2.3250000000000701E-5</v>
+        <v>0.72473919999999992</v>
       </c>
       <c r="J8" s="1">
         <f t="shared" si="3"/>
-        <v>4.000000000062981E-8</v>
+        <v>7.9830299999999993E-2</v>
       </c>
       <c r="K8" s="1">
         <f t="shared" si="4"/>
-        <v>2.339999999999981E-5</v>
+        <v>0.1825958</v>
       </c>
       <c r="L8" s="1">
         <f t="shared" si="5"/>
@@ -781,55 +781,55 @@
       </c>
       <c r="N8">
         <f t="shared" si="6"/>
-        <v>4.0017211703958591</v>
+        <v>4.0900195827243122</v>
       </c>
       <c r="O8">
         <f t="shared" si="0"/>
-        <v>4.0017211703958591</v>
-      </c>
-      <c r="P8" t="str">
+        <v>4.0900195827243122</v>
+      </c>
+      <c r="P8">
         <f t="shared" si="0"/>
-        <v/>
+        <v>4.9987664370695013</v>
       </c>
       <c r="Q8">
         <f t="shared" si="0"/>
-        <v>4.0137221269295926</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1.2359720544758077</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
-        <v>3.8000000000000002E-4</v>
+        <v>6.25E-2</v>
       </c>
       <c r="B9" s="1">
-        <v>-1.9876400000000002E-3</v>
+        <v>-0.33127299999999998</v>
       </c>
       <c r="C9" s="1">
-        <v>-1.9876400000000002E-3</v>
+        <v>-0.33127299999999998</v>
       </c>
       <c r="D9" s="1">
-        <v>-1.98183E-3</v>
+        <v>-0.170046</v>
       </c>
       <c r="E9" s="1">
-        <v>-1.9759999999999999E-3</v>
+        <v>-6.3414300000000003E-3</v>
       </c>
       <c r="F9" s="1">
-        <v>-1.98183E-3</v>
+        <v>-0.15407599999999999</v>
       </c>
       <c r="H9" s="1">
         <f t="shared" si="1"/>
-        <v>5.81000000000019E-6</v>
+        <v>0.17719699999999999</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="2"/>
-        <v>5.81000000000019E-6</v>
+        <v>0.17719699999999999</v>
       </c>
       <c r="J9" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1.5970000000000012E-2</v>
       </c>
       <c r="K9" s="1">
         <f t="shared" si="4"/>
-        <v>5.8300000000000712E-6</v>
+        <v>0.14773456999999998</v>
       </c>
       <c r="L9" s="1">
         <f t="shared" si="5"/>
@@ -837,55 +837,55 @@
       </c>
       <c r="N9">
         <f t="shared" si="6"/>
-        <v>4.0013774104687894</v>
+        <v>4.1535089775444183</v>
       </c>
       <c r="O9">
         <f t="shared" si="0"/>
-        <v>4.0013774104687894</v>
+        <v>4.1535089775444183</v>
       </c>
       <c r="P9">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6.7784380305602854</v>
       </c>
       <c r="Q9">
         <f t="shared" si="0"/>
-        <v>4.0096286107287264</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+        <v>3.2458079115905565</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
-        <v>1.9000000000000001E-4</v>
+        <v>3.125E-2</v>
       </c>
       <c r="B10" s="1">
-        <v>-9.9381899999999995E-4</v>
+        <v>-0.16563600000000001</v>
       </c>
       <c r="C10" s="1">
-        <v>-9.9381899999999995E-4</v>
+        <v>-0.16563600000000001</v>
       </c>
       <c r="D10" s="1">
-        <v>-9.9236799999999998E-4</v>
+        <v>-0.12533</v>
       </c>
       <c r="E10" s="1">
-        <v>-9.9091299999999995E-4</v>
+        <v>-7.74585E-2</v>
       </c>
       <c r="F10" s="1">
-        <v>-9.9236700000000008E-4</v>
+        <v>-0.122974</v>
       </c>
       <c r="H10" s="1">
         <f t="shared" si="1"/>
-        <v>1.451999999999877E-6</v>
+        <v>4.2662000000000005E-2</v>
       </c>
       <c r="I10" s="1">
         <f t="shared" si="2"/>
-        <v>1.451999999999877E-6</v>
+        <v>4.2662000000000005E-2</v>
       </c>
       <c r="J10" s="1">
         <f t="shared" si="3"/>
-        <v>9.9999999990732502E-10</v>
+        <v>2.355999999999997E-3</v>
       </c>
       <c r="K10" s="1">
         <f t="shared" si="4"/>
-        <v>1.4540000000001253E-6</v>
+        <v>4.55155E-2</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" si="5"/>
@@ -893,55 +893,55 @@
       </c>
       <c r="N10">
         <f t="shared" si="6"/>
-        <v>4</v>
+        <v>4.1049572781156218</v>
       </c>
       <c r="O10">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>4.1049572781156218</v>
       </c>
       <c r="P10">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>7.4533375514077793</v>
       </c>
       <c r="Q10">
         <f t="shared" si="0"/>
-        <v>4.0055096418727665</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+        <v>4.0443842189443755</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
-        <v>9.0000000000000006E-5</v>
+        <v>1.5630000000000002E-2</v>
       </c>
       <c r="B11" s="1">
-        <v>-4.9690900000000002E-4</v>
+        <v>-8.2818199999999995E-2</v>
       </c>
       <c r="C11" s="1">
-        <v>-4.9690900000000002E-4</v>
+        <v>-8.2818199999999995E-2</v>
       </c>
       <c r="D11" s="1">
-        <v>-4.9654699999999996E-4</v>
+        <v>-7.2741500000000001E-2</v>
       </c>
       <c r="E11" s="1">
-        <v>-4.9618299999999998E-4</v>
+        <v>-6.1171400000000001E-2</v>
       </c>
       <c r="F11" s="1">
-        <v>-4.9654600000000005E-4</v>
+        <v>-7.2425400000000001E-2</v>
       </c>
       <c r="H11" s="1">
         <f t="shared" si="1"/>
-        <v>3.6299999999996925E-7</v>
+        <v>1.0392799999999994E-2</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="2"/>
-        <v>3.6299999999996925E-7</v>
+        <v>1.0392799999999994E-2</v>
       </c>
       <c r="J11" s="1">
         <f t="shared" si="3"/>
-        <v>9.9999999990732502E-10</v>
+        <v>3.1609999999999971E-4</v>
       </c>
       <c r="K11" s="1">
         <f t="shared" si="4"/>
-        <v>3.6300000000007767E-7</v>
+        <v>1.1254E-2</v>
       </c>
       <c r="L11" s="1">
         <f t="shared" si="5"/>
@@ -949,55 +949,55 @@
       </c>
       <c r="N11">
         <f t="shared" si="6"/>
-        <v>3.9890109890096275</v>
+        <v>4.0596874999999981</v>
       </c>
       <c r="O11">
         <f t="shared" si="0"/>
-        <v>3.9890109890096275</v>
-      </c>
-      <c r="P11" t="str">
+        <v>4.0596874999999981</v>
+      </c>
+      <c r="P11">
         <f t="shared" si="0"/>
-        <v/>
+        <v>7.7475490196077299</v>
       </c>
       <c r="Q11">
         <f t="shared" si="0"/>
-        <v>3.9890109890131953</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+        <v>4.1696924786958132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
-        <v>5.0000000000000002E-5</v>
+        <v>7.8100000000000001E-3</v>
       </c>
       <c r="B12" s="1">
-        <v>-2.4845500000000002E-4</v>
+        <v>-4.1409099999999997E-2</v>
       </c>
       <c r="C12" s="1">
-        <v>-2.4845500000000002E-4</v>
+        <v>-4.1409099999999997E-2</v>
       </c>
       <c r="D12" s="1">
-        <v>-2.48364E-4</v>
+        <v>-3.8889899999999998E-2</v>
       </c>
       <c r="E12" s="1">
-        <v>-2.4827300000000003E-4</v>
+        <v>-3.6150099999999998E-2</v>
       </c>
       <c r="F12" s="1">
-        <v>-2.48364E-4</v>
+        <v>-3.8849099999999998E-2</v>
       </c>
       <c r="H12" s="1">
         <f t="shared" si="1"/>
-        <v>9.1000000000023354E-8</v>
+        <v>2.5599999999999998E-3</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="2"/>
-        <v>9.1000000000023354E-8</v>
+        <v>2.5599999999999998E-3</v>
       </c>
       <c r="J12" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>4.0800000000000558E-5</v>
       </c>
       <c r="K12" s="1">
         <f t="shared" si="4"/>
-        <v>9.0999999999969144E-8</v>
+        <v>2.699E-3</v>
       </c>
       <c r="L12" s="1">
         <f t="shared" si="5"/>
@@ -1005,55 +1005,55 @@
       </c>
       <c r="N12">
         <f t="shared" si="6"/>
-        <v>4.1363636363658207</v>
+        <v>4.031496062992125</v>
       </c>
       <c r="O12">
         <f t="shared" si="0"/>
-        <v>4.1363636363658207</v>
-      </c>
-      <c r="P12" t="str">
+        <v>4.031496062992125</v>
+      </c>
+      <c r="P12">
         <f t="shared" si="0"/>
-        <v/>
+        <v>7.8461538461534355</v>
       </c>
       <c r="Q12">
         <f t="shared" si="0"/>
-        <v>3.9565217391274117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+        <v>4.1250191043863671</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
-        <v>2.0000000000000002E-5</v>
+        <v>3.9100000000000003E-3</v>
       </c>
       <c r="B13" s="1">
-        <v>-1.24227E-4</v>
+        <v>-2.07046E-2</v>
       </c>
       <c r="C13" s="1">
-        <v>-1.24227E-4</v>
+        <v>-2.07046E-2</v>
       </c>
       <c r="D13" s="1">
-        <v>-1.2420500000000001E-4</v>
+        <v>-2.00748E-2</v>
       </c>
       <c r="E13" s="1">
-        <v>-1.24182E-4</v>
+        <v>-1.94153E-2</v>
       </c>
       <c r="F13" s="1">
-        <v>-1.2420500000000001E-4</v>
+        <v>-2.00696E-2</v>
       </c>
       <c r="H13" s="1">
         <f t="shared" si="1"/>
-        <v>2.199999999999403E-8</v>
+        <v>6.3500000000000015E-4</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" si="2"/>
-        <v>2.199999999999403E-8</v>
+        <v>6.3500000000000015E-4</v>
       </c>
       <c r="J13" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.2000000000003432E-6</v>
       </c>
       <c r="K13" s="1">
         <f t="shared" si="4"/>
-        <v>2.3000000000009775E-8</v>
+        <v>6.5430000000000002E-4</v>
       </c>
       <c r="L13" s="1">
         <f t="shared" si="5"/>
@@ -1061,55 +1061,55 @@
       </c>
       <c r="N13">
         <f t="shared" si="6"/>
-        <v>3.8596491228020953</v>
+        <v>4.0164452877925481</v>
       </c>
       <c r="O13">
         <f t="shared" si="0"/>
-        <v>3.8596491228020953</v>
-      </c>
-      <c r="P13" t="str">
+        <v>4.0164452877925481</v>
+      </c>
+      <c r="P13">
         <f t="shared" si="0"/>
-        <v/>
+        <v>8.6666666666685934</v>
       </c>
       <c r="Q13">
         <f t="shared" si="0"/>
-        <v>4.0350877193055039</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+        <v>4.0740971357409634</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
-        <v>1.0000000000000001E-5</v>
+        <v>1.9499999999999999E-3</v>
       </c>
       <c r="B14" s="1">
-        <v>-6.2113700000000001E-5</v>
+        <v>-1.03523E-2</v>
       </c>
       <c r="C14" s="1">
-        <v>-6.2113700000000001E-5</v>
+        <v>-1.03523E-2</v>
       </c>
       <c r="D14" s="1">
-        <v>-6.2107999999999996E-5</v>
+        <v>-1.01948E-2</v>
       </c>
       <c r="E14" s="1">
-        <v>-6.2102300000000003E-5</v>
+        <v>-1.00336E-2</v>
       </c>
       <c r="F14" s="1">
-        <v>-6.2107999999999996E-5</v>
+        <v>-1.01942E-2</v>
       </c>
       <c r="H14" s="1">
         <f t="shared" si="1"/>
-        <v>5.7000000000057222E-9</v>
+        <v>1.5809999999999956E-4</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="2"/>
-        <v>5.7000000000057222E-9</v>
+        <v>1.5809999999999956E-4</v>
       </c>
       <c r="J14" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>5.9999999999990616E-7</v>
       </c>
       <c r="K14" s="1">
         <f t="shared" si="4"/>
-        <v>5.6999999999921697E-9</v>
+        <v>1.6060000000000033E-4</v>
       </c>
       <c r="L14" s="1">
         <f t="shared" si="5"/>
@@ -1117,62 +1117,62 @@
       </c>
       <c r="N14">
         <f t="shared" si="6"/>
-        <v>4.0714285714434375</v>
+        <v>4.0076045627376411</v>
       </c>
       <c r="O14">
         <f t="shared" si="0"/>
-        <v>4.0714285714434375</v>
-      </c>
-      <c r="P14" t="str">
+        <v>4.0076045627376411</v>
+      </c>
+      <c r="P14">
         <f t="shared" si="0"/>
-        <v/>
+        <v>6.6666666667052157</v>
       </c>
       <c r="Q14">
         <f t="shared" si="0"/>
-        <v>4.0714285714140512</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+        <v>4.0392354124748779</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
-        <v>1.0000000000000001E-5</v>
+        <v>9.7999999999999997E-4</v>
       </c>
       <c r="B15" s="1">
-        <v>-3.1056799999999997E-5</v>
+        <v>-5.1761400000000001E-3</v>
       </c>
       <c r="C15" s="1">
-        <v>-3.1056799999999997E-5</v>
+        <v>-5.1761400000000001E-3</v>
       </c>
       <c r="D15" s="1">
-        <v>-3.1055400000000001E-5</v>
+        <v>-5.1367799999999996E-3</v>
       </c>
       <c r="E15" s="1">
-        <v>-3.1053999999999998E-5</v>
+        <v>-5.0969300000000004E-3</v>
       </c>
       <c r="F15" s="1">
-        <v>-3.1055400000000001E-5</v>
+        <v>-5.1366900000000002E-3</v>
       </c>
       <c r="H15" s="1">
         <f t="shared" si="1"/>
-        <v>1.3999999999962935E-9</v>
+        <v>3.9449999999999902E-5</v>
       </c>
       <c r="I15" s="1">
         <f t="shared" si="2"/>
-        <v>1.3999999999962935E-9</v>
+        <v>3.9449999999999902E-5</v>
       </c>
       <c r="J15" s="1">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8.9999999999465508E-8</v>
       </c>
       <c r="K15" s="1">
         <f t="shared" si="4"/>
-        <v>1.4000000000030698E-9</v>
+        <v>3.9759999999999796E-5</v>
       </c>
       <c r="L15" s="1">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A16" s="2"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1191,7 +1191,7 @@
       <c r="P16" s="7"/>
       <c r="Q16" s="7"/>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A17" s="2"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1205,22 +1205,22 @@
       <c r="L17" s="1"/>
       <c r="N17">
         <f>AVERAGE(N6:N14)</f>
-        <v>4.0087649241024996</v>
+        <v>3.7121122000561693</v>
       </c>
       <c r="O17">
         <f t="shared" ref="O17:Q17" si="7">AVERAGE(O6:O14)</f>
-        <v>4.0087649241024996</v>
+        <v>3.7121122000561693</v>
       </c>
       <c r="P17">
         <f t="shared" si="7"/>
-        <v>4.0452586206598022</v>
+        <v>14.283967049350801</v>
       </c>
       <c r="Q17">
         <f t="shared" si="7"/>
-        <v>4.0189114224653899</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+        <v>3.2310817809196575</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>7</v>
       </c>
@@ -1243,7 +1243,7 @@
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A20" s="4" t="s">
         <v>0</v>
       </c>
@@ -1290,40 +1290,40 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
-        <v>3.0000000000000001E-3</v>
+        <v>0.5</v>
       </c>
       <c r="B21" s="1">
-        <v>-2.4764499999999998E-3</v>
+        <v>-0.412742</v>
       </c>
       <c r="C21" s="1">
-        <v>-2.5241500000000002E-3</v>
+        <v>-1.73783</v>
       </c>
       <c r="D21" s="1">
-        <v>-2.5003E-3</v>
+        <v>-1.0752900000000001</v>
       </c>
       <c r="E21" s="1">
-        <v>-2.5218800000000002E-3</v>
+        <v>-6.6839700000000002E-2</v>
       </c>
       <c r="F21" s="1">
-        <v>-2.49993E-3</v>
+        <v>4.1189000000000003E-2</v>
       </c>
       <c r="H21" s="1">
         <f>ABS(B21-F21)</f>
-        <v>2.3480000000000202E-5</v>
+        <v>0.45393099999999997</v>
       </c>
       <c r="I21" s="1">
         <f>ABS(C21-F21)</f>
-        <v>2.4220000000000144E-5</v>
+        <v>1.7790189999999999</v>
       </c>
       <c r="J21" s="1">
         <f>ABS(D21-F21)</f>
-        <v>3.6999999999997105E-7</v>
+        <v>1.116479</v>
       </c>
       <c r="K21" s="1">
         <f>ABS(E21-F21)</f>
-        <v>2.1950000000000181E-5</v>
+        <v>0.10802870000000001</v>
       </c>
       <c r="L21" s="1">
         <f>ABS(F21-F21)</f>
@@ -1331,55 +1331,55 @@
       </c>
       <c r="N21">
         <f>IF(H22=0,"",H21/H22)</f>
-        <v>3.96621621621627</v>
+        <v>7.3808718557421829</v>
       </c>
       <c r="O21">
         <f t="shared" ref="O21:O29" si="8">IF(I22=0,"",I21/I22)</f>
-        <v>4.0299500831946418</v>
+        <v>4.5293705795190107</v>
       </c>
       <c r="P21">
         <f t="shared" ref="P21:P29" si="9">IF(J22=0,"",J21/J22)</f>
-        <v>7.3999999999791832</v>
+        <v>4.9154431026208858</v>
       </c>
       <c r="Q21">
         <f t="shared" ref="Q21:Q29" si="10">IF(K22=0,"",K21/K22)</f>
-        <v>3.8307155322862347</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1.5277214855124215</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
-        <v>1.5E-3</v>
+        <v>0.25</v>
       </c>
       <c r="B22" s="1">
-        <v>-1.2382199999999999E-3</v>
+        <v>-0.206371</v>
       </c>
       <c r="C22" s="1">
-        <v>-1.25015E-3</v>
+        <v>-0.53764400000000001</v>
       </c>
       <c r="D22" s="1">
-        <v>-1.2441900000000001E-3</v>
+        <v>-0.37200699999999998</v>
       </c>
       <c r="E22" s="1">
-        <v>-1.2498699999999999E-3</v>
+        <v>-7.4157699999999993E-2</v>
       </c>
       <c r="F22" s="1">
-        <v>-1.2441399999999999E-3</v>
+        <v>-0.14487</v>
       </c>
       <c r="H22" s="1">
         <f t="shared" ref="H22:H30" si="11">ABS(B22-F22)</f>
-        <v>5.9199999999999704E-6</v>
+        <v>6.1501E-2</v>
       </c>
       <c r="I22" s="1">
         <f t="shared" ref="I22:I30" si="12">ABS(C22-F22)</f>
-        <v>6.0100000000000865E-6</v>
+        <v>0.39277400000000001</v>
       </c>
       <c r="J22" s="1">
         <f t="shared" ref="J22:J30" si="13">ABS(D22-F22)</f>
-        <v>5.0000000000136741E-8</v>
+        <v>0.22713699999999998</v>
       </c>
       <c r="K22" s="1">
         <f t="shared" ref="K22:K30" si="14">ABS(E22-F22)</f>
-        <v>5.7300000000000146E-6</v>
+        <v>7.0712300000000006E-2</v>
       </c>
       <c r="L22" s="1">
         <f t="shared" ref="L22:L30" si="15">ABS(F22-F22)</f>
@@ -1387,55 +1387,55 @@
       </c>
       <c r="N22">
         <f t="shared" ref="N22:N29" si="16">IF(H23=0,"",H22/H23)</f>
-        <v>3.9865319865320661</v>
+        <v>5.3750218493270374</v>
       </c>
       <c r="O22">
         <f t="shared" si="8"/>
-        <v>4.0146960587841765</v>
+        <v>5.5028090281183015</v>
       </c>
       <c r="P22">
         <f t="shared" si="9"/>
-        <v>8.3333333333754975</v>
+        <v>7.5795708612807431</v>
       </c>
       <c r="Q22">
         <f t="shared" si="10"/>
-        <v>3.9192886456907523</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+        <v>1.6820162606267337</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
-        <v>7.5000000000000002E-4</v>
+        <v>0.125</v>
       </c>
       <c r="B23" s="1">
-        <v>-6.19112E-4</v>
+        <v>-0.103185</v>
       </c>
       <c r="C23" s="1">
-        <v>-6.2209400000000001E-4</v>
+        <v>-0.186004</v>
       </c>
       <c r="D23" s="1">
-        <v>-6.2060299999999995E-4</v>
+        <v>-0.144594</v>
       </c>
       <c r="E23" s="1">
-        <v>-6.22059E-4</v>
+        <v>-7.2586800000000007E-2</v>
       </c>
       <c r="F23" s="1">
-        <v>-6.2059699999999997E-4</v>
+        <v>-0.11462700000000001</v>
       </c>
       <c r="H23" s="1">
         <f t="shared" si="11"/>
-        <v>1.4849999999999629E-6</v>
+        <v>1.1442000000000008E-2</v>
       </c>
       <c r="I23" s="1">
         <f t="shared" si="12"/>
-        <v>1.4970000000000434E-6</v>
+        <v>7.1376999999999996E-2</v>
       </c>
       <c r="J23" s="1">
         <f t="shared" si="13"/>
-        <v>5.9999999999860512E-9</v>
+        <v>2.9966999999999994E-2</v>
       </c>
       <c r="K23" s="1">
         <f t="shared" si="14"/>
-        <v>1.4620000000000345E-6</v>
+        <v>4.20402E-2</v>
       </c>
       <c r="L23" s="1">
         <f t="shared" si="15"/>
@@ -1443,55 +1443,55 @@
       </c>
       <c r="N23">
         <f t="shared" si="16"/>
-        <v>3.991935483870841</v>
+        <v>1.7012355591239583</v>
       </c>
       <c r="O23">
         <f t="shared" si="8"/>
-        <v>4.0026737967917763</v>
+        <v>5.1060892208200963</v>
       </c>
       <c r="P23">
         <f t="shared" si="9"/>
-        <v>5.9999999998915801</v>
+        <v>8.2631114542546698</v>
       </c>
       <c r="Q23">
         <f t="shared" si="10"/>
-        <v>3.9620596205961971</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+        <v>6.6420513792776577</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
-        <v>3.8000000000000002E-4</v>
+        <v>6.25E-2</v>
       </c>
       <c r="B24" s="1">
-        <v>-3.09556E-4</v>
+        <v>-5.1592699999999998E-2</v>
       </c>
       <c r="C24" s="1">
-        <v>-3.1030199999999998E-4</v>
+        <v>-7.2297200000000006E-2</v>
       </c>
       <c r="D24" s="1">
-        <v>-3.0992900000000002E-4</v>
+        <v>-6.1945E-2</v>
       </c>
       <c r="E24" s="1">
-        <v>-3.1029700000000001E-4</v>
+        <v>-5.1989E-2</v>
       </c>
       <c r="F24" s="1">
-        <v>-3.09928E-4</v>
+        <v>-5.8318399999999999E-2</v>
       </c>
       <c r="H24" s="1">
         <f t="shared" si="11"/>
-        <v>3.7200000000000254E-7</v>
+        <v>6.7257000000000011E-3</v>
       </c>
       <c r="I24" s="1">
         <f t="shared" si="12"/>
-        <v>3.7399999999997982E-7</v>
+        <v>1.3978800000000006E-2</v>
       </c>
       <c r="J24" s="1">
         <f t="shared" si="13"/>
-        <v>1.0000000000157452E-9</v>
+        <v>3.6266000000000007E-3</v>
       </c>
       <c r="K24" s="1">
         <f t="shared" si="14"/>
-        <v>3.6900000000000951E-7</v>
+        <v>6.3293999999999989E-3</v>
       </c>
       <c r="L24" s="1">
         <f t="shared" si="15"/>
@@ -1499,55 +1499,55 @@
       </c>
       <c r="N24">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>3.1292513841715914</v>
       </c>
       <c r="O24">
         <f t="shared" si="8"/>
-        <v>4.0215053763438418</v>
-      </c>
-      <c r="P24" t="str">
+        <v>4.618190227625627</v>
+      </c>
+      <c r="P24">
         <f t="shared" si="9"/>
-        <v/>
+        <v>8.2648131267092158</v>
       </c>
       <c r="Q24">
         <f t="shared" si="10"/>
-        <v>3.967741935483946</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+        <v>23.329893107261448</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
-        <v>1.9000000000000001E-4</v>
+        <v>3.125E-2</v>
       </c>
       <c r="B25" s="1">
-        <v>-1.54778E-4</v>
+        <v>-2.5796300000000001E-2</v>
       </c>
       <c r="C25" s="1">
-        <v>-1.54964E-4</v>
+        <v>-3.09725E-2</v>
       </c>
       <c r="D25" s="1">
-        <v>-1.54871E-4</v>
+        <v>-2.8384400000000001E-2</v>
       </c>
       <c r="E25" s="1">
-        <v>-1.54964E-4</v>
+        <v>-2.82169E-2</v>
       </c>
       <c r="F25" s="1">
-        <v>-1.54871E-4</v>
+        <v>-2.7945600000000001E-2</v>
       </c>
       <c r="H25" s="1">
         <f t="shared" si="11"/>
-        <v>9.3000000000000634E-8</v>
+        <v>2.1492999999999998E-3</v>
       </c>
       <c r="I25" s="1">
         <f t="shared" si="12"/>
-        <v>9.3000000000000634E-8</v>
+        <v>3.026899999999999E-3</v>
       </c>
       <c r="J25" s="1">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>4.3879999999999961E-4</v>
       </c>
       <c r="K25" s="1">
         <f t="shared" si="14"/>
-        <v>9.3000000000000634E-8</v>
+        <v>2.7129999999999863E-4</v>
       </c>
       <c r="L25" s="1">
         <f t="shared" si="15"/>
@@ -1555,55 +1555,55 @@
       </c>
       <c r="N25">
         <f t="shared" si="16"/>
-        <v>3.9914163090122763</v>
+        <v>3.6226192482723762</v>
       </c>
       <c r="O25">
         <f t="shared" si="8"/>
-        <v>3.991416309014598</v>
-      </c>
-      <c r="P25" t="str">
+        <v>4.3198230341087456</v>
+      </c>
+      <c r="P25">
         <f t="shared" si="9"/>
-        <v/>
+        <v>8.171322160148927</v>
       </c>
       <c r="Q25">
         <f t="shared" si="10"/>
-        <v>3.991416309014598</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+        <v>0.74841379310344458</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
-        <v>9.0000000000000006E-5</v>
+        <v>1.5630000000000002E-2</v>
       </c>
       <c r="B26" s="1">
-        <v>-7.7389000000000001E-5</v>
+        <v>-1.28982E-2</v>
       </c>
       <c r="C26" s="1">
-        <v>-7.7435599999999994E-5</v>
+        <v>-1.41922E-2</v>
       </c>
       <c r="D26" s="1">
-        <v>-7.7412300000000004E-5</v>
+        <v>-1.35452E-2</v>
       </c>
       <c r="E26" s="1">
-        <v>-7.7435599999999994E-5</v>
+        <v>-1.3854E-2</v>
       </c>
       <c r="F26" s="1">
-        <v>-7.7412300000000004E-5</v>
+        <v>-1.34915E-2</v>
       </c>
       <c r="H26" s="1">
         <f t="shared" si="11"/>
-        <v>2.3300000000003656E-8</v>
+        <v>5.9329999999999973E-4</v>
       </c>
       <c r="I26" s="1">
         <f t="shared" si="12"/>
-        <v>2.3299999999990104E-8</v>
+        <v>7.0070000000000028E-4</v>
       </c>
       <c r="J26" s="1">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>5.3700000000000275E-5</v>
       </c>
       <c r="K26" s="1">
         <f t="shared" si="14"/>
-        <v>2.3299999999990104E-8</v>
+        <v>3.6249999999999998E-4</v>
       </c>
       <c r="L26" s="1">
         <f t="shared" si="15"/>
@@ -1611,55 +1611,55 @@
       </c>
       <c r="N26">
         <f t="shared" si="16"/>
-        <v>4.0172413793115531</v>
+        <v>3.8250273999097404</v>
       </c>
       <c r="O26">
         <f t="shared" si="8"/>
-        <v>3.9491525423716158</v>
-      </c>
-      <c r="P26" t="str">
+        <v>4.1611734663578606</v>
+      </c>
+      <c r="P26">
         <f t="shared" si="9"/>
-        <v/>
+        <v>8.0873493975908932</v>
       </c>
       <c r="Q26">
         <f t="shared" si="10"/>
-        <v>3.9491525423716158</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+        <v>2.8473804100227924</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
-        <v>5.0000000000000002E-5</v>
+        <v>7.8100000000000001E-3</v>
       </c>
       <c r="B27" s="1">
-        <v>-3.86945E-5</v>
+        <v>-6.4490900000000002E-3</v>
       </c>
       <c r="C27" s="1">
-        <v>-3.8706199999999999E-5</v>
+        <v>-6.7725900000000002E-3</v>
       </c>
       <c r="D27" s="1">
-        <v>-3.8700299999999999E-5</v>
+        <v>-6.6108399999999998E-3</v>
       </c>
       <c r="E27" s="1">
-        <v>-3.8706199999999999E-5</v>
+        <v>-6.7315099999999996E-3</v>
       </c>
       <c r="F27" s="1">
-        <v>-3.8700299999999999E-5</v>
+        <v>-6.6042000000000002E-3</v>
       </c>
       <c r="H27" s="1">
         <f t="shared" si="11"/>
-        <v>5.7999999999991652E-9</v>
+        <v>1.5510999999999997E-4</v>
       </c>
       <c r="I27" s="1">
         <f t="shared" si="12"/>
-        <v>5.8999999999993845E-9</v>
+        <v>1.6839000000000003E-4</v>
       </c>
       <c r="J27" s="1">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>6.6399999999995976E-6</v>
       </c>
       <c r="K27" s="1">
         <f t="shared" si="14"/>
-        <v>5.8999999999993845E-9</v>
+        <v>1.273099999999994E-4</v>
       </c>
       <c r="L27" s="1">
         <f t="shared" si="15"/>
@@ -1667,55 +1667,55 @@
       </c>
       <c r="N27">
         <f t="shared" si="16"/>
-        <v>4.1428571428574887</v>
+        <v>3.9149419485108763</v>
       </c>
       <c r="O27">
         <f t="shared" si="8"/>
-        <v>3.9333333333331826</v>
-      </c>
-      <c r="P27" t="str">
+        <v>4.0811924381968021</v>
+      </c>
+      <c r="P27">
         <f t="shared" si="9"/>
-        <v/>
+        <v>8.0975609756102465</v>
       </c>
       <c r="Q27">
         <f t="shared" si="10"/>
-        <v>3.9333333333331826</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+        <v>3.5149088901159415</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A28" s="2">
-        <v>2.0000000000000002E-5</v>
+        <v>3.9100000000000003E-3</v>
       </c>
       <c r="B28" s="1">
-        <v>-1.93473E-5</v>
+        <v>-3.2245400000000001E-3</v>
       </c>
       <c r="C28" s="1">
-        <v>-1.93502E-5</v>
+        <v>-3.3054199999999999E-3</v>
       </c>
       <c r="D28" s="1">
-        <v>-1.93487E-5</v>
+        <v>-3.2649799999999998E-3</v>
       </c>
       <c r="E28" s="1">
-        <v>-1.93502E-5</v>
+        <v>-3.3003799999999999E-3</v>
       </c>
       <c r="F28" s="1">
-        <v>-1.93487E-5</v>
+        <v>-3.2641599999999999E-3</v>
       </c>
       <c r="H28" s="1">
         <f t="shared" si="11"/>
-        <v>1.3999999999996817E-9</v>
+        <v>3.961999999999976E-5</v>
       </c>
       <c r="I28" s="1">
         <f t="shared" si="12"/>
-        <v>1.4999999999999009E-9</v>
+        <v>4.1259999999999995E-5</v>
       </c>
       <c r="J28" s="1">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>8.1999999999990067E-7</v>
       </c>
       <c r="K28" s="1">
         <f t="shared" si="14"/>
-        <v>1.4999999999999009E-9</v>
+        <v>3.6220000000000002E-5</v>
       </c>
       <c r="L28" s="1">
         <f t="shared" si="15"/>
@@ -1723,55 +1723,55 @@
       </c>
       <c r="N28">
         <f t="shared" si="16"/>
-        <v>3.8888888888904574</v>
+        <v>3.9580419580419473</v>
       </c>
       <c r="O28">
         <f t="shared" si="8"/>
-        <v>4.054054054048609</v>
-      </c>
-      <c r="P28" t="str">
+        <v>4.0411361410382511</v>
+      </c>
+      <c r="P28">
         <f t="shared" si="9"/>
-        <v/>
+        <v>8.1999999999943629</v>
       </c>
       <c r="Q28">
         <f t="shared" si="10"/>
-        <v>4.054054054048609</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+        <v>3.776850886339993</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A29" s="2">
-        <v>1.0000000000000001E-5</v>
+        <v>1.9499999999999999E-3</v>
       </c>
       <c r="B29" s="1">
-        <v>-9.6736300000000004E-6</v>
+        <v>-1.6122700000000001E-3</v>
       </c>
       <c r="C29" s="1">
-        <v>-9.6743600000000007E-6</v>
+        <v>-1.6324899999999999E-3</v>
       </c>
       <c r="D29" s="1">
-        <v>-9.6739900000000002E-6</v>
+        <v>-1.6223800000000001E-3</v>
       </c>
       <c r="E29" s="1">
-        <v>-9.6743600000000007E-6</v>
+        <v>-1.6318699999999999E-3</v>
       </c>
       <c r="F29" s="1">
-        <v>-9.6739900000000002E-6</v>
+        <v>-1.62228E-3</v>
       </c>
       <c r="H29" s="1">
         <f t="shared" si="11"/>
-        <v>3.5999999999977294E-10</v>
+        <v>1.0009999999999967E-5</v>
       </c>
       <c r="I29" s="1">
         <f t="shared" si="12"/>
-        <v>3.7000000000047249E-10</v>
+        <v>1.0209999999999863E-5</v>
       </c>
       <c r="J29" s="1">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1.0000000000005664E-7</v>
       </c>
       <c r="K29" s="1">
         <f t="shared" si="14"/>
-        <v>3.7000000000047249E-10</v>
+        <v>9.5899999999998591E-6</v>
       </c>
       <c r="L29" s="1">
         <f t="shared" si="15"/>
@@ -1779,55 +1779,55 @@
       </c>
       <c r="N29">
         <f t="shared" si="16"/>
-        <v>3.5999999999898358</v>
+        <v>3.981702466189482</v>
       </c>
       <c r="O29">
         <f t="shared" si="8"/>
-        <v>4.1111111111382996</v>
-      </c>
-      <c r="P29" t="str">
+        <v>4.0181031090121433</v>
+      </c>
+      <c r="P29">
         <f t="shared" si="9"/>
-        <v/>
+        <v>7.6923076922550857</v>
       </c>
       <c r="Q29">
         <f t="shared" si="10"/>
-        <v>4.1111111111382996</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+        <v>3.8936256597643397</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
-        <v>1.0000000000000001E-5</v>
+        <v>9.7999999999999997E-4</v>
       </c>
       <c r="B30" s="1">
-        <v>-4.8368099999999999E-6</v>
+        <v>-8.0613600000000005E-4</v>
       </c>
       <c r="C30" s="1">
-        <v>-4.8369999999999996E-6</v>
+        <v>-8.1119099999999995E-4</v>
       </c>
       <c r="D30" s="1">
-        <v>-4.8369100000000001E-6</v>
+        <v>-8.0866300000000005E-4</v>
       </c>
       <c r="E30" s="1">
-        <v>-4.8369999999999996E-6</v>
+        <v>-8.1111300000000002E-4</v>
       </c>
       <c r="F30" s="1">
-        <v>-4.8369100000000001E-6</v>
+        <v>-8.0864999999999995E-4</v>
       </c>
       <c r="H30" s="1">
         <f t="shared" si="11"/>
-        <v>1.0000000000021927E-10</v>
+        <v>2.5139999999999017E-6</v>
       </c>
       <c r="I30" s="1">
         <f t="shared" si="12"/>
-        <v>8.9999999999519718E-11</v>
+        <v>2.5410000000000016E-6</v>
       </c>
       <c r="J30" s="1">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1.3000000000096268E-8</v>
       </c>
       <c r="K30" s="1">
         <f t="shared" si="14"/>
-        <v>8.9999999999519718E-11</v>
+        <v>2.4630000000000745E-6</v>
       </c>
       <c r="L30" s="1">
         <f t="shared" si="15"/>
@@ -1835,7 +1835,7 @@
       </c>
       <c r="N30" s="9"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.45">
       <c r="H31" s="8" t="s">
         <v>11</v>
       </c>
@@ -1850,22 +1850,22 @@
       <c r="P31" s="7"/>
       <c r="Q31" s="7"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.45">
       <c r="H32" s="1">
         <f>(H21/ABS(F21))</f>
-        <v>9.3922629833636147E-3</v>
+        <v>11.020685134380537</v>
       </c>
       <c r="I32" s="1">
         <f>(I21/ABS(F21))</f>
-        <v>9.6882712715956627E-3</v>
+        <v>43.191604554614088</v>
       </c>
       <c r="J32" s="1">
         <f>(J21/ABS(F21))</f>
-        <v>1.4800414411602367E-4</v>
+        <v>27.106241957804265</v>
       </c>
       <c r="K32" s="1">
         <f>(K21/ABS(F21))</f>
-        <v>8.7802458468837843E-3</v>
+        <v>2.622756075651266</v>
       </c>
       <c r="L32" s="1">
         <f>(L21/ABS(F21))</f>
@@ -1873,220 +1873,220 @@
       </c>
       <c r="N32">
         <f>AVERAGE(N21:N29)</f>
-        <v>3.9538986007423094</v>
+        <v>4.0987459632543546</v>
       </c>
       <c r="O32">
         <f t="shared" ref="O32:Q32" si="17">AVERAGE(O21:O29)</f>
-        <v>4.0119880738911933</v>
+        <v>4.486431916088538</v>
       </c>
       <c r="P32">
         <f t="shared" si="17"/>
-        <v>7.2444444444154206</v>
+        <v>7.6968309744961134</v>
       </c>
       <c r="Q32">
         <f t="shared" si="17"/>
-        <v>3.9687636759959366</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+        <v>5.3292068746694197</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
       <c r="H33" s="1">
         <f t="shared" ref="H33:H41" si="18">(H22/ABS(F22))</f>
-        <v>4.7583069429485191E-3</v>
+        <v>0.42452543659832953</v>
       </c>
       <c r="I33" s="1">
         <f t="shared" ref="I33:I41" si="19">(I22/ABS(F22))</f>
-        <v>4.8306460687704651E-3</v>
+        <v>2.7112169531303927</v>
       </c>
       <c r="J33" s="1">
         <f t="shared" ref="J33:J41" si="20">(J22/ABS(F22))</f>
-        <v>4.0188403234472602E-5</v>
+        <v>1.567867743494167</v>
       </c>
       <c r="K33" s="1">
         <f t="shared" ref="K33:K41" si="21">(K22/ABS(F22))</f>
-        <v>4.6055910106579763E-3</v>
+        <v>0.48810864913370611</v>
       </c>
       <c r="L33" s="1">
         <f t="shared" ref="L33:L41" si="22">(L22/ABS(F22))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
       <c r="H34" s="1">
         <f t="shared" si="18"/>
-        <v>2.3928572004053563E-3</v>
+        <v>9.9819414274123955E-2</v>
       </c>
       <c r="I34" s="1">
         <f t="shared" si="19"/>
-        <v>2.4121934202067422E-3</v>
+        <v>0.62268924424437522</v>
       </c>
       <c r="J34" s="1">
         <f t="shared" si="20"/>
-        <v>9.6681099006054682E-6</v>
+        <v>0.2614305530110706</v>
       </c>
       <c r="K34" s="1">
         <f t="shared" si="21"/>
-        <v>2.3557961124530645E-3</v>
+        <v>0.36675652333219921</v>
       </c>
       <c r="L34" s="1">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
       <c r="H35" s="1">
         <f t="shared" si="18"/>
-        <v>1.200278774425036E-3</v>
+        <v>0.11532723805865733</v>
       </c>
       <c r="I35" s="1">
         <f t="shared" si="19"/>
-        <v>1.2067318861154197E-3</v>
+        <v>0.23969793409970105</v>
       </c>
       <c r="J35" s="1">
         <f t="shared" si="20"/>
-        <v>3.2265558452793722E-6</v>
+        <v>6.2186205382863742E-2</v>
       </c>
       <c r="K35" s="1">
         <f t="shared" si="21"/>
-        <v>1.1905991068893727E-3</v>
+        <v>0.10853178413673899</v>
       </c>
       <c r="L35" s="1">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
       <c r="H36" s="1">
         <f t="shared" si="18"/>
-        <v>6.0049977077697328E-4</v>
+        <v>7.6910139699988542E-2</v>
       </c>
       <c r="I36" s="1">
         <f t="shared" si="19"/>
-        <v>6.0049977077697328E-4</v>
+        <v>0.10831401007672045</v>
       </c>
       <c r="J36" s="1">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>1.5701935188365955E-2</v>
       </c>
       <c r="K36" s="1">
         <f t="shared" si="21"/>
-        <v>6.0049977077697328E-4</v>
+        <v>9.7081472575288631E-3</v>
       </c>
       <c r="L36" s="1">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
       <c r="H37" s="1">
         <f t="shared" si="18"/>
-        <v>3.0098576066082077E-4</v>
+        <v>4.3975836637883091E-2</v>
       </c>
       <c r="I37" s="1">
         <f t="shared" si="19"/>
-        <v>3.0098576066064567E-4</v>
+        <v>5.1936404402772134E-2</v>
       </c>
       <c r="J37" s="1">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>3.9802838824445222E-3</v>
       </c>
       <c r="K37" s="1">
         <f t="shared" si="21"/>
-        <v>3.0098576066064567E-4</v>
+        <v>2.6868769225067632E-2</v>
       </c>
       <c r="L37" s="1">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
       <c r="H38" s="1">
         <f t="shared" si="18"/>
-        <v>1.4986963925342091E-4</v>
+        <v>2.3486569152963259E-2</v>
       </c>
       <c r="I38" s="1">
         <f t="shared" si="19"/>
-        <v>1.5245359855089972E-4</v>
+        <v>2.5497410738620881E-2</v>
       </c>
       <c r="J38" s="1">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>1.0054207928287449E-3</v>
       </c>
       <c r="K38" s="1">
         <f t="shared" si="21"/>
-        <v>1.5245359855089972E-4</v>
+        <v>1.9277126676963054E-2</v>
       </c>
       <c r="L38" s="1">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
       <c r="H39" s="1">
         <f t="shared" si="18"/>
-        <v>7.235628233419721E-5</v>
+        <v>1.2137885397774545E-2</v>
       </c>
       <c r="I39" s="1">
         <f t="shared" si="19"/>
-        <v>7.7524588215223815E-5</v>
+        <v>1.2640311749424047E-2</v>
       </c>
       <c r="J39" s="1">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>2.5121317582468404E-4</v>
       </c>
       <c r="K39" s="1">
         <f t="shared" si="21"/>
-        <v>7.7524588215223815E-5</v>
+        <v>1.1096269790696535E-2</v>
       </c>
       <c r="L39" s="1">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
       <c r="H40" s="1">
         <f t="shared" si="18"/>
-        <v>3.7213187113049831E-5</v>
+        <v>6.1703281800921956E-3</v>
       </c>
       <c r="I40" s="1">
         <f t="shared" si="19"/>
-        <v>3.8246886755151959E-5</v>
+        <v>6.2936114604136544E-3</v>
       </c>
       <c r="J40" s="1">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>6.1641640160796309E-5</v>
       </c>
       <c r="K40" s="1">
         <f t="shared" si="21"/>
-        <v>3.8246886755151959E-5</v>
+        <v>5.9114332914169312E-3</v>
       </c>
       <c r="L40" s="1">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
       <c r="H41" s="1">
         <f t="shared" si="18"/>
-        <v>2.0674356148908968E-5</v>
+        <v>3.1088851790019192E-3</v>
       </c>
       <c r="I41" s="1">
         <f t="shared" si="19"/>
-        <v>1.8606920533877976E-5</v>
+        <v>3.1422741606381027E-3</v>
       </c>
       <c r="J41" s="1">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>1.6076176343407246E-5</v>
       </c>
       <c r="K41" s="1">
         <f t="shared" si="21"/>
-        <v>1.8606920533877976E-5</v>
+        <v>3.0458171025784637E-3</v>
       </c>
       <c r="L41" s="1">
         <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
       <c r="H42" s="11" t="s">
         <v>12</v>
       </c>
@@ -2095,43 +2095,43 @@
       <c r="K42" s="10"/>
       <c r="L42" s="10"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
       <c r="H43" s="1">
         <f>AVERAGE(H32:H41)</f>
-        <v>1.8925304897429896E-3</v>
+        <v>1.1826146867559353</v>
       </c>
       <c r="I43" s="1">
         <f t="shared" ref="I43:K43" si="23">AVERAGE(I32:I41)</f>
-        <v>1.9326160172181063E-3</v>
+        <v>4.6973032708677147</v>
       </c>
       <c r="J43" s="1">
         <f t="shared" si="23"/>
-        <v>2.0108721309638108E-5</v>
+        <v>2.901874303054834</v>
       </c>
       <c r="K43" s="1">
         <f t="shared" si="23"/>
-        <v>1.8120549602376975E-3</v>
+        <v>0.36620605955981611</v>
       </c>
       <c r="L43" s="1">
         <f>AVERAGE(L32:L41)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.45">
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.45">
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A46" s="3" t="s">
         <v>14</v>
       </c>
@@ -2148,7 +2148,7 @@
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A47" s="16" t="s">
         <v>0</v>
       </c>
@@ -2183,264 +2183,264 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A48" s="2">
-        <v>3.0000000000000001E-3</v>
+        <v>1E-3</v>
       </c>
       <c r="B48" s="1">
-        <v>2.5208200000000001</v>
+        <v>2.2577400000000001</v>
       </c>
       <c r="C48" s="1">
-        <v>2.1962100000000002</v>
+        <v>2.1962000000000002</v>
       </c>
       <c r="D48" s="1">
-        <v>2.1962299999999999</v>
+        <v>2.1962000000000002</v>
       </c>
       <c r="E48" s="1">
-        <v>2.1916899999999999</v>
+        <v>2.1946699999999999</v>
       </c>
       <c r="F48" s="1">
-        <v>2.0000399999999998</v>
+        <v>2</v>
       </c>
       <c r="H48" s="1">
         <f>IF(B48="inf","inf",ABS(B48-F48))</f>
-        <v>0.52078000000000024</v>
+        <v>0.25774000000000008</v>
       </c>
       <c r="I48" s="1">
         <f>IF(C48="inf","inf",ABS(C48-F48))</f>
-        <v>0.1961700000000004</v>
+        <v>0.19620000000000015</v>
       </c>
       <c r="J48" s="1">
         <f>IF(D48="inf","inf",ABS(D48-F48))</f>
-        <v>0.19619000000000009</v>
+        <v>0.19620000000000015</v>
       </c>
       <c r="K48" s="1">
         <f>IF(E48="inf","inf",ABS(E48-F48))</f>
-        <v>0.1916500000000001</v>
+        <v>0.1946699999999999</v>
       </c>
       <c r="L48" s="1">
         <f>IF(F48="inf","inf",ABS(F48-F48))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A49" s="2">
-        <v>6.0000000000000001E-3</v>
+        <v>2E-3</v>
       </c>
       <c r="B49" s="1">
-        <v>22.305299999999999</v>
+        <v>2.8079900000000002</v>
       </c>
       <c r="C49" s="1">
-        <v>2.19624</v>
+        <v>2.1962000000000002</v>
       </c>
       <c r="D49" s="1">
-        <v>2.1967099999999999</v>
+        <v>2.1962199999999998</v>
       </c>
       <c r="E49" s="1">
-        <v>2.1874199999999999</v>
+        <v>2.1931699999999998</v>
       </c>
       <c r="F49" s="1">
-        <v>2.0001799999999998</v>
+        <v>2.0000200000000001</v>
       </c>
       <c r="H49" s="1">
         <f t="shared" ref="H49:H57" si="24">IF(B49="inf","inf",ABS(B49-F49))</f>
-        <v>20.305119999999999</v>
+        <v>0.80797000000000008</v>
       </c>
       <c r="I49" s="1">
         <f t="shared" ref="I49:I57" si="25">IF(C49="inf","inf",ABS(C49-F49))</f>
-        <v>0.19606000000000012</v>
+        <v>0.19618000000000002</v>
       </c>
       <c r="J49" s="1">
         <f t="shared" ref="J49:J57" si="26">IF(D49="inf","inf",ABS(D49-F49))</f>
-        <v>0.19653000000000009</v>
+        <v>0.19619999999999971</v>
       </c>
       <c r="K49" s="1">
         <f t="shared" ref="K49:K57" si="27">IF(E49="inf","inf",ABS(E49-F49))</f>
-        <v>0.18724000000000007</v>
+        <v>0.19314999999999971</v>
       </c>
       <c r="L49" s="1">
         <f t="shared" ref="L49:L57" si="28">IF(F49="inf","inf",ABS(F49-F49))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A50" s="2">
-        <v>1.2E-2</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="B50" s="1">
-        <v>1135900000</v>
+        <v>288.05399999999997</v>
       </c>
       <c r="C50" s="1">
-        <v>2.19638</v>
+        <v>2.1962199999999998</v>
       </c>
       <c r="D50" s="1">
-        <v>2.2050000000000001</v>
+        <v>2.19651</v>
       </c>
       <c r="E50" s="1">
-        <v>2.1795100000000001</v>
+        <v>2.1902499999999998</v>
       </c>
       <c r="F50" s="1">
-        <v>2.0007100000000002</v>
+        <v>2.0000800000000001</v>
       </c>
       <c r="H50" s="1">
         <f t="shared" si="24"/>
-        <v>1135899997.99929</v>
+        <v>286.05391999999995</v>
       </c>
       <c r="I50" s="1">
         <f t="shared" si="25"/>
-        <v>0.19566999999999979</v>
+        <v>0.19613999999999976</v>
       </c>
       <c r="J50" s="1">
         <f t="shared" si="26"/>
-        <v>0.20428999999999986</v>
+        <v>0.19642999999999988</v>
       </c>
       <c r="K50" s="1">
         <f t="shared" si="27"/>
-        <v>0.17879999999999985</v>
+        <v>0.19016999999999973</v>
       </c>
       <c r="L50" s="1">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A51" s="2">
-        <v>2.4E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="B51" s="1">
-        <v>1.91731E+39</v>
+        <v>6905780000000</v>
       </c>
       <c r="C51" s="1">
-        <v>2.1969099999999999</v>
+        <v>2.1962799999999998</v>
       </c>
       <c r="D51" s="1">
-        <v>2.4876100000000001</v>
+        <v>2.2012900000000002</v>
       </c>
       <c r="E51" s="1">
-        <v>2.1660499999999998</v>
+        <v>2.1846899999999998</v>
       </c>
       <c r="F51" s="1">
-        <v>2.0028100000000002</v>
+        <v>2.0003099999999998</v>
       </c>
       <c r="H51" s="1">
         <f t="shared" si="24"/>
-        <v>1.91731E+39</v>
+        <v>6905779999998</v>
       </c>
       <c r="I51" s="1">
         <f t="shared" si="25"/>
-        <v>0.19409999999999972</v>
+        <v>0.19596999999999998</v>
       </c>
       <c r="J51" s="1">
         <f t="shared" si="26"/>
-        <v>0.4847999999999999</v>
+        <v>0.20098000000000038</v>
       </c>
       <c r="K51" s="1">
         <f t="shared" si="27"/>
-        <v>0.16323999999999961</v>
+        <v>0.18437999999999999</v>
       </c>
       <c r="L51" s="1">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A52" s="2">
-        <v>4.8000000000000001E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="B52" s="1">
-        <v>2.9498900000000001E+148</v>
+        <v>7.6071499999999996E+53</v>
       </c>
       <c r="C52" s="1">
-        <v>2.1991499999999999</v>
+        <v>2.19652</v>
       </c>
       <c r="D52" s="1">
-        <v>329248000</v>
+        <v>2.3203999999999998</v>
       </c>
       <c r="E52" s="1">
-        <v>2.1455799999999998</v>
+        <v>2.1746300000000001</v>
       </c>
       <c r="F52" s="1">
-        <v>2.0110899999999998</v>
+        <v>2.0012500000000002</v>
       </c>
       <c r="H52" s="1">
         <f t="shared" si="24"/>
-        <v>2.9498900000000001E+148</v>
+        <v>7.6071499999999996E+53</v>
       </c>
       <c r="I52" s="1">
         <f t="shared" si="25"/>
-        <v>0.18806000000000012</v>
+        <v>0.19526999999999983</v>
       </c>
       <c r="J52" s="1">
         <f t="shared" si="26"/>
-        <v>329247997.98891002</v>
+        <v>0.3191499999999996</v>
       </c>
       <c r="K52" s="1">
         <f t="shared" si="27"/>
-        <v>0.13449</v>
+        <v>0.17337999999999987</v>
       </c>
       <c r="L52" s="1">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A53" s="2">
-        <v>9.6000000000000002E-2</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>15</v>
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="B53" s="1">
+        <v>4.0725800000000002E+210</v>
       </c>
       <c r="C53" s="1">
-        <v>2.2099199999999999</v>
+        <v>2.1974800000000001</v>
       </c>
       <c r="D53" s="1">
-        <v>1.27972E+138</v>
+        <v>47226.9</v>
       </c>
       <c r="E53" s="1">
-        <v>2.1245799999999999</v>
+        <v>2.15829</v>
       </c>
       <c r="F53" s="1">
-        <v>2.0418400000000001</v>
-      </c>
-      <c r="H53" s="1" t="str">
+        <v>2.0049800000000002</v>
+      </c>
+      <c r="H53" s="1">
         <f t="shared" si="24"/>
-        <v>inf</v>
+        <v>4.0725800000000002E+210</v>
       </c>
       <c r="I53" s="1">
         <f t="shared" si="25"/>
-        <v>0.16807999999999979</v>
+        <v>0.19249999999999989</v>
       </c>
       <c r="J53" s="1">
         <f t="shared" si="26"/>
-        <v>1.27972E+138</v>
+        <v>47224.895020000004</v>
       </c>
       <c r="K53" s="1">
         <f t="shared" si="27"/>
-        <v>8.2739999999999814E-2</v>
+        <v>0.15330999999999984</v>
       </c>
       <c r="L53" s="1">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A54" s="2">
-        <v>0.192</v>
+        <v>6.4000000000000001E-2</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C54" s="1">
-        <v>2.4484599999999999</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>15</v>
+        <v>2.2016399999999998</v>
+      </c>
+      <c r="D54" s="1">
+        <v>1.51951E+88</v>
       </c>
       <c r="E54" s="1">
-        <v>2.1101000000000001</v>
+        <v>2.1378900000000001</v>
       </c>
       <c r="F54" s="1">
-        <v>2.1316600000000001</v>
+        <v>2.0194100000000001</v>
       </c>
       <c r="H54" s="1" t="str">
         <f t="shared" si="24"/>
@@ -2448,47 +2448,47 @@
       </c>
       <c r="I54" s="1">
         <f t="shared" si="25"/>
-        <v>0.31679999999999975</v>
-      </c>
-      <c r="J54" s="1" t="str">
+        <v>0.18222999999999967</v>
+      </c>
+      <c r="J54" s="1">
         <f t="shared" si="26"/>
-        <v>inf</v>
+        <v>1.51951E+88</v>
       </c>
       <c r="K54" s="1">
         <f t="shared" si="27"/>
-        <v>2.1560000000000024E-2</v>
+        <v>0.11847999999999992</v>
       </c>
       <c r="L54" s="1">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A55" s="2">
-        <v>0.38400000000000001</v>
+        <v>0.128</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>15</v>
+      <c r="C55" s="1">
+        <v>2.2257699999999998</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>15</v>
       </c>
       <c r="E55" s="1">
-        <v>2.1035400000000002</v>
+        <v>2.1190099999999998</v>
       </c>
       <c r="F55" s="1">
-        <v>2.1732300000000002</v>
+        <v>2.0699700000000001</v>
       </c>
       <c r="H55" s="1" t="str">
         <f t="shared" si="24"/>
         <v>inf</v>
       </c>
-      <c r="I55" s="1" t="str">
+      <c r="I55" s="1">
         <f t="shared" si="25"/>
-        <v>inf</v>
+        <v>0.15579999999999972</v>
       </c>
       <c r="J55" s="1" t="str">
         <f t="shared" si="26"/>
@@ -2496,16 +2496,16 @@
       </c>
       <c r="K55" s="1">
         <f t="shared" si="27"/>
-        <v>6.969000000000003E-2</v>
+        <v>4.903999999999975E-2</v>
       </c>
       <c r="L55" s="1">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A56" s="2">
-        <v>0.76800000000000002</v>
+        <v>0.25600000000000001</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>15</v>
@@ -2514,13 +2514,13 @@
         <v>15</v>
       </c>
       <c r="D56" s="1">
-        <v>1.5059099999999999E+307</v>
+        <v>6.8823199999999995E+306</v>
       </c>
       <c r="E56" s="1">
-        <v>2.0996800000000002</v>
+        <v>2.10765</v>
       </c>
       <c r="F56" s="1">
-        <v>2.0811199999999999</v>
+        <v>2.1800700000000002</v>
       </c>
       <c r="H56" s="1" t="str">
         <f t="shared" si="24"/>
@@ -2532,20 +2532,20 @@
       </c>
       <c r="J56" s="1">
         <f t="shared" si="26"/>
-        <v>1.5059099999999999E+307</v>
+        <v>6.8823199999999995E+306</v>
       </c>
       <c r="K56" s="1">
         <f t="shared" si="27"/>
-        <v>1.8560000000000354E-2</v>
+        <v>7.2420000000000151E-2</v>
       </c>
       <c r="L56" s="1">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A57" s="2">
-        <v>1.536</v>
+        <v>0.51200000000000001</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>15</v>
@@ -2553,14 +2553,14 @@
       <c r="C57" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D57" s="1">
-        <v>3.9737399999999998E+307</v>
+      <c r="D57" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="E57" s="1">
-        <v>2.0985100000000001</v>
+        <v>2.1014400000000002</v>
       </c>
       <c r="F57" s="1">
-        <v>2.1903199999999998</v>
+        <v>2.0592100000000002</v>
       </c>
       <c r="H57" s="1" t="str">
         <f t="shared" si="24"/>
@@ -2570,20 +2570,20 @@
         <f t="shared" si="25"/>
         <v>inf</v>
       </c>
-      <c r="J57" s="1">
+      <c r="J57" s="1" t="str">
         <f t="shared" si="26"/>
-        <v>3.9737399999999998E+307</v>
+        <v>inf</v>
       </c>
       <c r="K57" s="1">
         <f t="shared" si="27"/>
-        <v>9.1809999999999725E-2</v>
+        <v>4.222999999999999E-2</v>
       </c>
       <c r="L57" s="1">
         <f t="shared" si="28"/>
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.45">
       <c r="H58" s="8" t="s">
         <v>11</v>
       </c>
@@ -2592,168 +2592,168 @@
       <c r="K58" s="7"/>
       <c r="L58" s="7"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.45">
       <c r="H59" s="1">
         <f>IF(H48="inf","inf",(H48/ABS(F48)))</f>
-        <v>0.26038479230415407</v>
+        <v>0.12887000000000004</v>
       </c>
       <c r="I59" s="1">
         <f>IF(I48="inf","inf",(I48/ABS(F48)))</f>
-        <v>9.808303833923343E-2</v>
+        <v>9.8100000000000076E-2</v>
       </c>
       <c r="J59" s="1">
         <f>IF(J48="inf","inf",(J48/ABS(F48)))</f>
-        <v>9.8093038139237268E-2</v>
+        <v>9.8100000000000076E-2</v>
       </c>
       <c r="K59" s="1">
         <f>IF(K48="inf","inf",(K48/ABS(F48)))</f>
-        <v>9.5823083538329287E-2</v>
+        <v>9.7334999999999949E-2</v>
       </c>
       <c r="L59" s="1">
         <f>IF(L48="inf","inf",(L48/ABS(F48)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.45">
       <c r="H60" s="1">
         <f t="shared" ref="H60:H68" si="29">IF(H49="inf","inf",(H49/ABS(F49)))</f>
-        <v>10.151646351828335</v>
+        <v>0.40398096019039809</v>
       </c>
       <c r="I60" s="1">
         <f t="shared" ref="I60:I68" si="30">IF(I49="inf","inf",(I49/ABS(F49)))</f>
-        <v>9.8021178093971609E-2</v>
+        <v>9.8089019109808911E-2</v>
       </c>
       <c r="J60" s="1">
         <f t="shared" ref="J60:J68" si="31">IF(J49="inf","inf",(J49/ABS(F49)))</f>
-        <v>9.8256156945874931E-2</v>
+        <v>9.8099019009809746E-2</v>
       </c>
       <c r="K60" s="1">
         <f t="shared" ref="K60:K68" si="32">IF(K49="inf","inf",(K49/ABS(F49)))</f>
-        <v>9.3611574958253799E-2</v>
+        <v>9.6574034259657257E-2</v>
       </c>
       <c r="L60" s="1">
         <f t="shared" ref="L60:L68" si="33">IF(L49="inf","inf",(L49/ABS(F49)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.45">
       <c r="H61" s="1">
         <f t="shared" si="29"/>
-        <v>567748448.30049825</v>
+        <v>143.02123915043396</v>
       </c>
       <c r="I61" s="1">
         <f t="shared" si="30"/>
-        <v>9.7800280900280284E-2</v>
+        <v>9.8066077356905604E-2</v>
       </c>
       <c r="J61" s="1">
         <f t="shared" si="31"/>
-        <v>0.10210875139325531</v>
+        <v>9.8211071557137652E-2</v>
       </c>
       <c r="K61" s="1">
         <f t="shared" si="32"/>
-        <v>8.9368274262636674E-2</v>
+        <v>9.5081196752129782E-2</v>
       </c>
       <c r="L61" s="1">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.45">
       <c r="H62" s="1">
         <f t="shared" si="29"/>
-        <v>9.5730997947883217E+38</v>
+        <v>3452354884991.8267</v>
       </c>
       <c r="I62" s="1">
         <f t="shared" si="30"/>
-        <v>9.6913836060335073E-2</v>
+        <v>9.7969814678724801E-2</v>
       </c>
       <c r="J62" s="1">
         <f t="shared" si="31"/>
-        <v>0.24205990583230552</v>
+        <v>0.1004744264638983</v>
       </c>
       <c r="K62" s="1">
         <f t="shared" si="32"/>
-        <v>8.1505484793864422E-2</v>
+        <v>9.2175712764521509E-2</v>
       </c>
       <c r="L62" s="1">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.45">
       <c r="H63" s="1">
         <f t="shared" si="29"/>
-        <v>1.4668115300657854E+148</v>
+        <v>3.8011992504684568E+53</v>
       </c>
       <c r="I63" s="1">
         <f t="shared" si="30"/>
-        <v>9.3511478849778049E-2</v>
+        <v>9.757401623985E-2</v>
       </c>
       <c r="J63" s="1">
         <f t="shared" si="31"/>
-        <v>163716192.70590082</v>
+        <v>0.15947532792004976</v>
       </c>
       <c r="K63" s="1">
         <f t="shared" si="32"/>
-        <v>6.687418265716602E-2</v>
+        <v>8.6635852592129844E-2</v>
       </c>
       <c r="L63" s="1">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="H64" s="1" t="str">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="H64" s="1">
         <f t="shared" si="29"/>
-        <v>inf</v>
+        <v>2.03123223174296E+210</v>
       </c>
       <c r="I64" s="1">
         <f t="shared" si="30"/>
-        <v>8.2317909336676612E-2</v>
+        <v>9.6010932777384247E-2</v>
       </c>
       <c r="J64" s="1">
         <f t="shared" si="31"/>
-        <v>6.2674842299102769E+137</v>
+        <v>23553.798551606498</v>
       </c>
       <c r="K64" s="1">
         <f t="shared" si="32"/>
-        <v>4.0522274027347788E-2</v>
+        <v>7.646460313818583E-2</v>
       </c>
       <c r="L64" s="1">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="8:12" x14ac:dyDescent="0.45">
       <c r="H65" s="1" t="str">
         <f t="shared" si="29"/>
         <v>inf</v>
       </c>
       <c r="I65" s="1">
         <f t="shared" si="30"/>
-        <v>0.14861657112297447</v>
-      </c>
-      <c r="J65" s="1" t="str">
+        <v>9.0239228289450704E-2</v>
+      </c>
+      <c r="J65" s="1">
         <f t="shared" si="31"/>
-        <v>inf</v>
+        <v>7.5245244898262361E+87</v>
       </c>
       <c r="K65" s="1">
         <f t="shared" si="32"/>
-        <v>1.0114183312535781E-2</v>
+        <v>5.8670601809439345E-2</v>
       </c>
       <c r="L65" s="1">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="8:12" x14ac:dyDescent="0.45">
       <c r="H66" s="1" t="str">
         <f t="shared" si="29"/>
         <v>inf</v>
       </c>
-      <c r="I66" s="1" t="str">
+      <c r="I66" s="1">
         <f t="shared" si="30"/>
-        <v>inf</v>
+        <v>7.526679130615406E-2</v>
       </c>
       <c r="J66" s="1" t="str">
         <f t="shared" si="31"/>
@@ -2761,14 +2761,14 @@
       </c>
       <c r="K66" s="1">
         <f t="shared" si="32"/>
-        <v>3.2067475600833791E-2</v>
+        <v>2.369116460625021E-2</v>
       </c>
       <c r="L66" s="1">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="8:12" x14ac:dyDescent="0.45">
       <c r="H67" s="1" t="str">
         <f t="shared" si="29"/>
         <v>inf</v>
@@ -2779,18 +2779,18 @@
       </c>
       <c r="J67" s="1">
         <f t="shared" si="31"/>
-        <v>7.236055585453986E+306</v>
+        <v>3.1569261537473565E+306</v>
       </c>
       <c r="K67" s="1">
         <f t="shared" si="32"/>
-        <v>8.9182747751212592E-3</v>
+        <v>3.3219116817349965E-2</v>
       </c>
       <c r="L67" s="1">
         <f t="shared" si="33"/>
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="8:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="8:12" x14ac:dyDescent="0.45">
       <c r="H68" s="1" t="str">
         <f t="shared" si="29"/>
         <v>inf</v>
@@ -2799,13 +2799,13 @@
         <f t="shared" si="30"/>
         <v>inf</v>
       </c>
-      <c r="J68" s="1">
+      <c r="J68" s="1" t="str">
         <f t="shared" si="31"/>
-        <v>1.8142280580006574E+307</v>
+        <v>inf</v>
       </c>
       <c r="K68" s="1">
         <f t="shared" si="32"/>
-        <v>4.1916249680411875E-2</v>
+        <v>2.0507864666546874E-2</v>
       </c>
       <c r="L68" s="1">
         <f t="shared" si="33"/>

</xml_diff>